<commit_message>
Updated some frame parts. Still need to update everything after the frame is finished.
</commit_message>
<xml_diff>
--- a/DIN Rail layout.xlsx
+++ b/DIN Rail layout.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="135" windowWidth="19155" windowHeight="11310"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
   <si>
     <t>GND</t>
   </si>
@@ -73,13 +73,19 @@
   </si>
   <si>
     <t>Relay</t>
+  </si>
+  <si>
+    <t>Jumper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">throui </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,7 +127,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -279,11 +285,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -296,12 +315,18 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -380,6 +405,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -414,6 +440,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -589,181 +616,279 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>6</v>
+      </c>
+      <c r="D1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>24</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>24</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>24</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C7" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>3</v>
+      <c r="B8" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C13" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="9" t="s">
+      <c r="D13">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B14" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>13.8</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>13.8</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>13.8</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="D18">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="2">
-        <v>13.8</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="2">
-        <v>13.8</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="2">
-        <v>13.8</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="D19">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -773,24 +898,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated DIN Rail layout with revised positions/status.
</commit_message>
<xml_diff>
--- a/DIN Rail layout.xlsx
+++ b/DIN Rail layout.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="135" windowWidth="19155" windowHeight="11310"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
   <si>
     <t>GND</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Sense</t>
   </si>
   <si>
-    <t>Batttery -</t>
-  </si>
-  <si>
     <t>E-stop</t>
   </si>
   <si>
@@ -78,14 +75,23 @@
     <t>Jumper</t>
   </si>
   <si>
-    <t xml:space="preserve">throui </t>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Battery -</t>
+  </si>
+  <si>
+    <t>Router</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,6 +102,26 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF92D050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -158,7 +184,7 @@
         <color theme="0"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color theme="0"/>
       </top>
       <bottom style="thin">
         <color theme="0"/>
@@ -173,7 +199,7 @@
         <color theme="0"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color theme="0"/>
       </top>
       <bottom style="thin">
         <color theme="0"/>
@@ -188,7 +214,7 @@
         <color indexed="64"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color theme="0"/>
       </top>
       <bottom style="thin">
         <color theme="0"/>
@@ -206,7 +232,7 @@
         <color theme="0"/>
       </top>
       <bottom style="thin">
-        <color theme="0"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -215,85 +241,77 @@
         <color theme="0"/>
       </left>
       <right style="thin">
-        <color theme="0"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
         <color theme="0"/>
       </top>
       <bottom style="thin">
-        <color theme="0"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color theme="0"/>
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
-        <color theme="0"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top style="thin">
-        <color theme="0"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0"/>
-      </left>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top style="thin">
-        <color theme="0"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color theme="0"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0"/>
-      </left>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top style="thin">
-        <color theme="0"/>
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -302,20 +320,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -617,278 +644,280 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>24</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="D1">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>24</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="D2">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>24</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>19</v>
+      <c r="B3" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>24</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="1"/>
+      <c r="B4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>1</v>
+      </c>
       <c r="D4">
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>24</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="B5" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="9"/>
       <c r="D5">
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>24</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D6">
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="5" t="s">
+      <c r="B7" s="12" t="s">
         <v>4</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D7">
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>5</v>
+      <c r="B8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="D8">
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="8"/>
+        <v>18</v>
+      </c>
+      <c r="C9" s="4"/>
       <c r="D9">
         <v>85</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="L9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="8"/>
+        <v>18</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>12</v>
+      </c>
       <c r="D10">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="8"/>
+      <c r="C11" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="D13">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>15</v>
+      <c r="B14" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>8</v>
       </c>
       <c r="D14">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>13.8</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>13</v>
+      <c r="B15" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>8</v>
       </c>
       <c r="D15">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>13.8</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>14</v>
+      <c r="B16" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>10</v>
       </c>
       <c r="D16">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>13.8</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17">
+        <v>30</v>
+      </c>
+      <c r="G17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>12</v>
+      <c r="B18" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>7</v>
       </c>
       <c r="D18">
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>7</v>
+      <c r="C19" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="D19">
         <v>85</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D20" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>